<commit_message>
(E-16): Copy ready xlsx file to output directory and remove temp directory
</commit_message>
<xml_diff>
--- a/src/resources/template.xlsx
+++ b/src/resources/template.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">Update type</t>
   </si>
   <si>
-    <t xml:space="preserve">Proirity</t>
+    <t xml:space="preserve">Priority</t>
   </si>
   <si>
     <t xml:space="preserve">Comment</t>
@@ -61,6 +61,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -82,6 +83,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -150,9 +152,15 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -273,16 +281,16 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.98"/>
   </cols>
   <sheetData>

</xml_diff>